<commit_message>
Update results of test case 20160404 - 002
</commit_message>
<xml_diff>
--- a/20160404 - 002/running_logs/logs.xlsx
+++ b/20160404 - 002/running_logs/logs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="26">
   <si>
     <t>Time</t>
   </si>
@@ -71,6 +71,27 @@
   </si>
   <si>
     <t>20160405_093759</t>
+  </si>
+  <si>
+    <t>20160405_102700</t>
+  </si>
+  <si>
+    <t>convert to lower, convert unicode to ascii, remove multiple spaces, trim "space" and ","</t>
+  </si>
+  <si>
+    <t>2 layers: [100-Sigmoid, 3-Softmax], learning_rate: 0.01, learning_rule: adagrad, n_iterator: 300</t>
+  </si>
+  <si>
+    <t>20160405_103113</t>
+  </si>
+  <si>
+    <t>20160405_103522</t>
+  </si>
+  <si>
+    <t>20160405_103956</t>
+  </si>
+  <si>
+    <t>20160405_104604</t>
   </si>
 </sst>
 </file>
@@ -402,7 +423,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -597,6 +618,166 @@
         <v>0.163265306122449</v>
       </c>
     </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>253.297</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7">
+        <v>0.979333333333333</v>
+      </c>
+      <c r="H7">
+        <v>0.996699669966997</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7">
+        <v>0.13265306122449</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>249.092</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8">
+        <v>0.974666666666667</v>
+      </c>
+      <c r="H8">
+        <v>0.996699669966997</v>
+      </c>
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8">
+        <v>0.142857142857143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>273.641</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9">
+        <v>0.971333333333333</v>
+      </c>
+      <c r="H9">
+        <v>0.996699669966997</v>
+      </c>
+      <c r="I9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9">
+        <v>0.183673469387755</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>368.064</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10">
+        <v>0.977333333333333</v>
+      </c>
+      <c r="H10">
+        <v>0.996699669966997</v>
+      </c>
+      <c r="I10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10">
+        <v>0.122448979591837</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11">
+        <v>494.456</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11">
+        <v>0.974</v>
+      </c>
+      <c r="H11">
+        <v>0.996699669966997</v>
+      </c>
+      <c r="I11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11">
+        <v>0.153061224489796</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>